<commit_message>
Added guidenotes & resource links
</commit_message>
<xml_diff>
--- a/Project 3 Prototype/Revenue data/state_data_combined_revenue.xlsx
+++ b/Project 3 Prototype/Revenue data/state_data_combined_revenue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8af7e8536f9e44ec/Desktop/Project 3 Data/Revenue data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8af7e8536f9e44ec/Desktop/Data Bootcamp/Project-3-Sports-Betting-Analysis/Project 3 Prototype/Revenue data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{6770E7CA-7A49-4C10-8AC5-1B8CDF330F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92B67E56-AED7-4AC7-A325-FB99584DE99D}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{6770E7CA-7A49-4C10-8AC5-1B8CDF330F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4139B4C1-168F-45D0-9FFA-987FCA6B2601}"/>
   <bookViews>
-    <workbookView xWindow="72570" yWindow="1095" windowWidth="22980" windowHeight="10710" xr2:uid="{33C7E7ED-9421-46C4-9E1B-653A366B1C20}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{33C7E7ED-9421-46C4-9E1B-653A366B1C20}"/>
   </bookViews>
   <sheets>
     <sheet name="All States" sheetId="1" r:id="rId1"/>
@@ -212,10 +212,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -547,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4F6735-3E98-456D-B1B8-D26994589A5B}">
   <dimension ref="A1:F1098"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -557,7 +553,7 @@
     <col min="2" max="2" width="10.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.61328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.07421875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3828125" customWidth="1"/>
+    <col min="5" max="5" width="20.3046875" customWidth="1"/>
     <col min="6" max="6" width="20.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>